<commit_message>
Corrección tablas, importación y exportación
</commit_message>
<xml_diff>
--- a/MateriasPrimas.xlsx
+++ b/MateriasPrimas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaavi\Documents\laCartaDeNanaYRene\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AC0A45-E688-4DF7-B4AB-BA6ACD167976}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85038B7D-A4FD-4F46-AC28-E26CE737912B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{52233312-3386-4175-B67F-D59C803E40A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{52233312-3386-4175-B67F-D59C803E40A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>harina</t>
   </si>
@@ -48,19 +48,10 @@
     <t>crema</t>
   </si>
   <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t>unidades</t>
-  </si>
-  <si>
     <t>Nombre</t>
   </si>
   <si>
     <t>Cantidad</t>
-  </si>
-  <si>
-    <t>Unidad de medida</t>
   </si>
 </sst>
 </file>
@@ -412,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6D5BE5-992D-4217-ADE3-FBC8960037E6}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,70 +414,52 @@
     <col min="3" max="3" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>